<commit_message>
Added data extraction method to plates and slabs; need to add this to plate torques module though.
There is an error in the rms velocity calculation.

Net rotation needs to be updated after calculating synthetic stage rotations.
</commit_message>
<xml_diff>
--- a/tests/cases_test.xlsx
+++ b/tests/cases_test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/project/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thomas/Documents/_Plato/Plato/tests/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFA74A06-490D-8F43-B488-D80D224224DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BD6594-7CF8-0C4D-BB36-94A68D3E5304}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16260" xr2:uid="{0A9D0FCF-1F4B-5247-B35D-CBB46409C9D9}"/>
   </bookViews>
@@ -59,7 +59,7 @@
     <t>Reconstructed motions</t>
   </si>
   <si>
-    <t>sediment thickness</t>
+    <t>sediment_thickness</t>
   </si>
 </sst>
 </file>
@@ -434,7 +434,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>